<commit_message>
POST June 9 2016 meeting
</commit_message>
<xml_diff>
--- a/misc_docs/OMOP_concept_for_smoking.xlsx
+++ b/misc_docs/OMOP_concept_for_smoking.xlsx
@@ -9,18 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="2" r:id="rId1"/>
     <sheet name="OMOP Convention for Smoke" sheetId="4" r:id="rId2"/>
+    <sheet name="Reduced set" sheetId="5" r:id="rId3"/>
+    <sheet name="Map" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <definedNames>
+    <definedName name="SMOKING">Map!$F$3:$F$13</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="131">
   <si>
     <t>Description</t>
   </si>
@@ -317,6 +322,102 @@
   </si>
   <si>
     <t>How many years did you smoke up to now [PhenX]</t>
+  </si>
+  <si>
+    <t>How many years did you smoke up to now</t>
+  </si>
+  <si>
+    <t>Very heavy cigarette smoker (40+ cigs/day)</t>
+  </si>
+  <si>
+    <t>Trivial cigarette smoker (less than one cigarette/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex-moderate cigarette smoker (10-19/day) </t>
+  </si>
+  <si>
+    <t>Reduced set of values</t>
+  </si>
+  <si>
+    <t>OMOP Values</t>
+  </si>
+  <si>
+    <t>SMOKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01=Current every day smoker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02=Current some day smoker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03=Former smoker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04=Never smoker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">05=Smoker, current status unknown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">06=Unknown if ever smoked </t>
+  </si>
+  <si>
+    <t xml:space="preserve">07=Heavy tobacco smoker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">08=Light tobacco smoker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NI=No information </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN=Unknown </t>
+  </si>
+  <si>
+    <t>OT=Other</t>
+  </si>
+  <si>
+    <t>TOBACCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01=Current user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02=Never </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03=Quit/former user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04=Passive or environmental exposure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">06=Not asked </t>
+  </si>
+  <si>
+    <t>TOBACCO_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01=Smoked tobacco only </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02=Non-smoked tobacco only </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03=Use of both smoked and non-smoked tobacco products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04=None </t>
+  </si>
+  <si>
+    <t xml:space="preserve">05=Use of smoked tobacco but no information about non-smoked tobacco use </t>
+  </si>
+  <si>
+    <t>UN=Unknow</t>
+  </si>
+  <si>
+    <t>Possible OMOP values</t>
   </si>
 </sst>
 </file>
@@ -722,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -787,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,4 +1508,858 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="F9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="F13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="F15" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="F16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="F17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="F19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="F21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="F25" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="F26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="F27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="F29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:A44">
+    <sortCondition ref="A2:A44"/>
+  </sortState>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B29">
+      <formula1>SMOKING</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29">
+      <formula1>$F$16:$F$23</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D29">
+      <formula1>$F$26:$F$32</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>$F$26:$F$33</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>